<commit_message>
remove button response automation
</commit_message>
<xml_diff>
--- a/exp/trials/twoafc_practice_trials.xlsx
+++ b/exp/trials/twoafc_practice_trials.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -357,16 +357,6 @@
           <t>correct_response</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>prac_button_si</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>prac_button_no</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -377,16 +367,6 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -397,16 +377,6 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -417,16 +387,6 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -437,16 +397,6 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -457,16 +407,6 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -477,16 +417,6 @@
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -497,16 +427,6 @@
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -516,16 +436,6 @@
       </c>
       <c r="B9">
         <v>0</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Sí</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>